<commit_message>
re-added the function in manage reservation
</commit_message>
<xml_diff>
--- a/public/test.xlsx
+++ b/public/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>driver_name</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>uploads/fleet_management/users/FMD-644D125E/1682772574_imansyah-muhamad-putera-n4KewLKFOZw-unsplash.jpg</t>
+  </si>
+  <si>
+    <t>l0gistic@!</t>
+  </si>
+  <si>
+    <t>2023-05-03 20:52:50</t>
+  </si>
+  <si>
+    <t>uploads/fleet_management/users/FMD-64525922/1683118370_christian_aliwate.jpg</t>
   </si>
 </sst>
 </file>
@@ -414,7 +423,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,6 +506,32 @@
         <v>19</v>
       </c>
       <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>